<commit_message>
dataManagement adding scoring for totals, highlighting on codebook
</commit_message>
<xml_diff>
--- a/codebook/smarvus_codebook_250124.xlsx
+++ b/codebook/smarvus_codebook_250124.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarst\Documents\GitHub\2301\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1E9F45-CB75-461D-A8AA-041FDDA51FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E885AE8-9E19-4B5C-B47C-4E752DD832AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6730" yWindow="0" windowWidth="19320" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="29340" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -6732,7 +6732,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6775,6 +6775,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -6788,7 +6794,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -6816,24 +6822,26 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7071,8 +7079,11 @@
   </sheetPr>
   <dimension ref="A1:AA1014"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A473" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B490" sqref="B490"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7087,52 +7098,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>2115</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
     </row>
     <row r="2" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="21" t="s">
         <v>1868</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="23" t="s">
         <v>1869</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="21" t="s">
         <v>4</v>
       </c>
       <c r="L2" s="1"/>
@@ -7153,17 +7164,17 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -7181,13 +7192,13 @@
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" spans="1:27" s="18" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:27" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:27" s="19" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+    <row r="5" spans="1:27" s="20" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
         <v>10</v>
       </c>
     </row>
@@ -7195,7 +7206,7 @@
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -7497,8 +7508,8 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" spans="1:27" s="19" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+    <row r="12" spans="1:27" s="20" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
         <v>23</v>
       </c>
     </row>
@@ -7706,8 +7717,8 @@
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
     </row>
-    <row r="17" spans="1:27" s="19" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="19" t="s">
+    <row r="17" spans="1:27" s="20" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
         <v>36</v>
       </c>
     </row>
@@ -8101,8 +8112,8 @@
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
     </row>
-    <row r="26" spans="1:27" s="19" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="19" t="s">
+    <row r="26" spans="1:27" s="20" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="20" t="s">
         <v>71</v>
       </c>
     </row>
@@ -8251,8 +8262,8 @@
       <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
     </row>
-    <row r="30" spans="1:27" s="19" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="19" t="s">
+    <row r="30" spans="1:27" s="20" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="20" t="s">
         <v>82</v>
       </c>
     </row>
@@ -8305,8 +8316,8 @@
       <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
     </row>
-    <row r="32" spans="1:27" s="19" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="19" t="s">
+    <row r="32" spans="1:27" s="20" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="20" t="s">
         <v>87</v>
       </c>
     </row>
@@ -9493,7 +9504,7 @@
       <c r="C56" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" s="25" t="s">
         <v>1907</v>
       </c>
       <c r="E56" s="1" t="s">
@@ -11737,7 +11748,7 @@
       <c r="C100" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D100" s="1" t="s">
+      <c r="D100" s="25" t="s">
         <v>1907</v>
       </c>
       <c r="E100" s="1" t="s">
@@ -14020,7 +14031,7 @@
       <c r="C146" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D146" s="1" t="s">
+      <c r="D146" s="25" t="s">
         <v>1907</v>
       </c>
       <c r="E146" s="1" t="s">
@@ -15652,7 +15663,7 @@
       <c r="C180" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D180" s="1" t="s">
+      <c r="D180" s="25" t="s">
         <v>1907</v>
       </c>
       <c r="E180" s="1" t="s">
@@ -17620,7 +17631,7 @@
       <c r="C221" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D221" s="1" t="s">
+      <c r="D221" s="25" t="s">
         <v>1907</v>
       </c>
       <c r="E221" s="1" t="s">
@@ -18628,7 +18639,7 @@
       <c r="C242" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D242" s="1" t="s">
+      <c r="D242" s="25" t="s">
         <v>1907</v>
       </c>
       <c r="E242" s="1" t="s">
@@ -19563,8 +19574,8 @@
       <c r="Z260" s="1"/>
       <c r="AA260" s="1"/>
     </row>
-    <row r="261" spans="1:27" s="19" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A261" s="19" t="s">
+    <row r="261" spans="1:27" s="20" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A261" s="20" t="s">
         <v>593</v>
       </c>
     </row>
@@ -29513,8 +29524,8 @@
       <c r="Z456" s="1"/>
       <c r="AA456" s="1"/>
     </row>
-    <row r="457" spans="1:27" s="19" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A457" s="19" t="s">
+    <row r="457" spans="1:27" s="20" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A457" s="20" t="s">
         <v>842</v>
       </c>
     </row>
@@ -29525,7 +29536,7 @@
       <c r="B458" t="s">
         <v>2078</v>
       </c>
-      <c r="C458" s="23" t="s">
+      <c r="C458" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D458" s="1" t="s">
@@ -29572,7 +29583,7 @@
       <c r="B459" t="s">
         <v>2079</v>
       </c>
-      <c r="C459" s="23" t="s">
+      <c r="C459" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D459" s="1" t="s">
@@ -29621,7 +29632,7 @@
       <c r="B460" t="s">
         <v>2080</v>
       </c>
-      <c r="C460" s="23" t="s">
+      <c r="C460" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D460" s="1" t="s">
@@ -29670,7 +29681,7 @@
       <c r="B461" t="s">
         <v>2081</v>
       </c>
-      <c r="C461" s="23" t="s">
+      <c r="C461" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D461" s="1" t="s">
@@ -29719,7 +29730,7 @@
       <c r="B462" t="s">
         <v>2082</v>
       </c>
-      <c r="C462" s="23" t="s">
+      <c r="C462" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D462" s="1" t="s">
@@ -29768,7 +29779,7 @@
       <c r="B463" t="s">
         <v>2083</v>
       </c>
-      <c r="C463" s="23" t="s">
+      <c r="C463" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D463" s="1" t="s">
@@ -29817,7 +29828,7 @@
       <c r="B464" t="s">
         <v>2084</v>
       </c>
-      <c r="C464" s="23" t="s">
+      <c r="C464" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D464" s="1" t="s">
@@ -29866,7 +29877,7 @@
       <c r="B465" t="s">
         <v>2085</v>
       </c>
-      <c r="C465" s="23" t="s">
+      <c r="C465" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D465" s="1" t="s">
@@ -29915,7 +29926,7 @@
       <c r="B466" s="4" t="s">
         <v>859</v>
       </c>
-      <c r="C466" s="23" t="s">
+      <c r="C466" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D466" s="1" t="s">
@@ -29964,7 +29975,7 @@
       <c r="B467" t="s">
         <v>861</v>
       </c>
-      <c r="C467" s="23" t="s">
+      <c r="C467" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D467" s="1" t="s">
@@ -30013,7 +30024,7 @@
       <c r="B468" t="s">
         <v>864</v>
       </c>
-      <c r="C468" s="23" t="s">
+      <c r="C468" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D468" s="1" t="s">
@@ -30062,7 +30073,7 @@
       <c r="B469" t="s">
         <v>867</v>
       </c>
-      <c r="C469" s="23" t="s">
+      <c r="C469" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D469" s="1" t="s">
@@ -30111,7 +30122,7 @@
       <c r="B470" t="s">
         <v>870</v>
       </c>
-      <c r="C470" s="23" t="s">
+      <c r="C470" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D470" s="1" t="s">
@@ -30160,7 +30171,7 @@
       <c r="B471" t="s">
         <v>873</v>
       </c>
-      <c r="C471" s="23" t="s">
+      <c r="C471" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D471" s="1" t="s">
@@ -30209,7 +30220,7 @@
       <c r="B472" t="s">
         <v>875</v>
       </c>
-      <c r="C472" s="23" t="s">
+      <c r="C472" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D472" s="1" t="s">
@@ -30258,7 +30269,7 @@
       <c r="B473" s="4" t="s">
         <v>2088</v>
       </c>
-      <c r="C473" s="23" t="s">
+      <c r="C473" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D473" s="1" t="s">
@@ -30307,7 +30318,7 @@
       <c r="B474" s="4" t="s">
         <v>2090</v>
       </c>
-      <c r="C474" s="23" t="s">
+      <c r="C474" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D474" s="1" t="s">
@@ -30356,7 +30367,7 @@
       <c r="B475" s="4" t="s">
         <v>2096</v>
       </c>
-      <c r="C475" s="23" t="s">
+      <c r="C475" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D475" s="1" t="s">
@@ -30405,7 +30416,7 @@
       <c r="B476" t="s">
         <v>2097</v>
       </c>
-      <c r="C476" s="23" t="s">
+      <c r="C476" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D476" s="1" t="s">
@@ -30454,7 +30465,7 @@
       <c r="B477" t="s">
         <v>2098</v>
       </c>
-      <c r="C477" s="23" t="s">
+      <c r="C477" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D477" s="1" t="s">
@@ -30503,7 +30514,7 @@
       <c r="B478" t="s">
         <v>2099</v>
       </c>
-      <c r="C478" s="23" t="s">
+      <c r="C478" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D478" s="1" t="s">
@@ -30552,7 +30563,7 @@
       <c r="B479" t="s">
         <v>2100</v>
       </c>
-      <c r="C479" s="23" t="s">
+      <c r="C479" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D479" s="1" t="s">
@@ -30601,7 +30612,7 @@
       <c r="B480" t="s">
         <v>2101</v>
       </c>
-      <c r="C480" s="23" t="s">
+      <c r="C480" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D480" s="1" t="s">
@@ -30650,7 +30661,7 @@
       <c r="B481" t="s">
         <v>2102</v>
       </c>
-      <c r="C481" s="23" t="s">
+      <c r="C481" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D481" s="1" t="s">
@@ -30699,7 +30710,7 @@
       <c r="B482" t="s">
         <v>2110</v>
       </c>
-      <c r="C482" s="23" t="s">
+      <c r="C482" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D482" s="1" t="s">
@@ -30748,7 +30759,7 @@
       <c r="B483" s="1" t="s">
         <v>1479</v>
       </c>
-      <c r="C483" s="23" t="s">
+      <c r="C483" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D483" s="1" t="s">
@@ -30792,8 +30803,8 @@
       <c r="Z483" s="1"/>
       <c r="AA483" s="1"/>
     </row>
-    <row r="484" spans="1:27" s="18" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A484" s="18" t="s">
+    <row r="484" spans="1:27" s="19" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A484" s="19" t="s">
         <v>2034</v>
       </c>
     </row>
@@ -31208,7 +31219,7 @@
       <c r="F493" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G493" s="24" t="s">
+      <c r="G493" s="17" t="s">
         <v>1599</v>
       </c>
       <c r="H493" s="1" t="s">
@@ -45691,8 +45702,8 @@
       <c r="Z796" s="1"/>
       <c r="AA796" s="1"/>
     </row>
-    <row r="797" spans="1:27" s="18" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A797" s="18" t="s">
+    <row r="797" spans="1:27" s="19" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A797" s="19" t="s">
         <v>2033</v>
       </c>
     </row>
@@ -45703,7 +45714,7 @@
       <c r="B798" s="1" t="s">
         <v>1475</v>
       </c>
-      <c r="C798" s="23" t="s">
+      <c r="C798" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D798" s="1" t="s">
@@ -45752,7 +45763,7 @@
       <c r="B799" s="1" t="s">
         <v>1476</v>
       </c>
-      <c r="C799" s="23" t="s">
+      <c r="C799" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D799" s="1" t="s">
@@ -45803,7 +45814,7 @@
       <c r="B800" s="1" t="s">
         <v>2094</v>
       </c>
-      <c r="C800" s="23" t="s">
+      <c r="C800" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D800" s="1" t="s">
@@ -45854,7 +45865,7 @@
       <c r="B801" s="1" t="s">
         <v>2095</v>
       </c>
-      <c r="C801" s="23" t="s">
+      <c r="C801" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D801" s="1" t="s">
@@ -45905,7 +45916,7 @@
       <c r="B802" s="1" t="s">
         <v>2091</v>
       </c>
-      <c r="C802" s="23" t="s">
+      <c r="C802" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D802" s="1" t="s">
@@ -52098,7 +52109,14 @@
       <c r="AA1014" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="22">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A797:XFD797"/>
     <mergeCell ref="A484:XFD484"/>
@@ -52110,18 +52128,10 @@
     <mergeCell ref="A26:XFD26"/>
     <mergeCell ref="A17:XFD17"/>
     <mergeCell ref="A5:XFD5"/>
-    <mergeCell ref="A4:XFD4"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>